<commit_message>
just for test -> updates on readme.md
</commit_message>
<xml_diff>
--- a/Results/SpreadSheets/Device.xlsx
+++ b/Results/SpreadSheets/Device.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="12552" windowHeight="4536" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="12552" windowHeight="4536"/>
   </bookViews>
   <sheets>
     <sheet name="OverallDevicePieChart" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -150,6 +149,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -159,6 +159,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:dLbls>
+            <c:showCatName val="1"/>
             <c:showPercent val="1"/>
             <c:showLeaderLines val="1"/>
           </c:dLbls>
@@ -241,24 +242,12 @@
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:showCatName val="1"/>
           <c:showPercent val="1"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900"/>
-          </a:pPr>
-          <a:endParaRPr lang="tr-TR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
 </c:chartSpace>
@@ -354,24 +343,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="100565376"/>
-        <c:axId val="100566912"/>
+        <c:axId val="92909952"/>
+        <c:axId val="92911488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="100565376"/>
+        <c:axId val="92909952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100566912"/>
+        <c:crossAx val="92911488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100566912"/>
+        <c:axId val="92911488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -379,7 +368,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100565376"/>
+        <c:crossAx val="92909952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -414,7 +403,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -542,7 +530,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -632,25 +619,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="107436672"/>
-        <c:axId val="107442560"/>
+        <c:axId val="94514560"/>
+        <c:axId val="94528640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="107436672"/>
+        <c:axId val="94514560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107442560"/>
+        <c:crossAx val="94528640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107442560"/>
+        <c:axId val="94528640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,7 +651,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="107436672"/>
+        <c:crossAx val="94514560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -678,7 +665,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -689,7 +676,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="62" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1215,7 +1202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18763"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>

</xml_diff>